<commit_message>
write to template successful
</commit_message>
<xml_diff>
--- a/src/main/resources/sample/excel/Mock.xlsx
+++ b/src/main/resources/sample/excel/Mock.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khair\Documents\GitHub\repositories\rendr\src\main\resources\sample\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Desktop\repos\Rendr\src\main\resources\sample\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF009347-65DA-4A07-AD80-293A56E52CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0C320C-5A2B-48C0-8E4E-131D600E9205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="1155" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2772" yWindow="2772" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataInputs" sheetId="7" r:id="rId1"/>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Total Redemptions (Includes Interest and Dividend Income)</t>
-  </si>
-  <si>
-    <t>Days</t>
   </si>
   <si>
     <t>Current Month-End Market Capitalization</t>
@@ -53,16 +50,13 @@
     <t>assetName</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>compositionRate</t>
   </si>
   <si>
-    <t>currentMonthNAV</t>
+    <t>groupAccount</t>
   </si>
   <si>
-    <t>groupAccount</t>
+    <t>blanktest</t>
   </si>
 </sst>
 </file>
@@ -710,7 +704,7 @@
     <xf numFmtId="38" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -727,9 +721,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="38" fontId="30" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="30" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1170,226 +1161,197 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449881BD-6A68-49C0-AA20-83DAB95B90EE}">
   <dimension ref="B6:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1"/>
+    <col min="1" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="14.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.75" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:13">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="2:13">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="2:13" ht="14.45" customHeight="1">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="9" spans="2:13" ht="63.75">
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="H9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
     </row>
     <row r="10" spans="2:13">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
     </row>
     <row r="11" spans="2:13">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" spans="2:13">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13" spans="2:13">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="14" spans="2:13">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1404,27 +1366,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BCDC333-A2EA-4E11-B848-97C032B08655}">
   <dimension ref="C9:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="5.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.25" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="3:6" ht="63.75">
+    <row r="9" spans="3:6" ht="25.5">
       <c r="C9" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>6</v>
+      <c r="F9" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="3:6">
@@ -1457,21 +1425,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008CDC787A71DDF645B3B1EC4B4C087709" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfcc5dabae62faba7569d214b4f3e22c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -1585,7 +1538,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835BF43D-5F5B-4A92-8B6A-74ACA0EB3617}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31452BF2-B3C4-4EBE-BE76-B62708FA3B9D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1600,26 +1584,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA689A5-2DDE-4193-801A-F36D3E40FA78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835BF43D-5F5B-4A92-8B6A-74ACA0EB3617}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
function in template works after writing
</commit_message>
<xml_diff>
--- a/src/main/resources/sample/excel/Mock.xlsx
+++ b/src/main/resources/sample/excel/Mock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Desktop\repos\Rendr\src\main\resources\sample\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0C320C-5A2B-48C0-8E4E-131D600E9205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB170604-84B5-4953-9D63-66659CCE548E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2772" yWindow="2772" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataInputs" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Total Redemptions (Includes Interest and Dividend Income)</t>
   </si>
@@ -58,6 +58,15 @@
   <si>
     <t>blanktest</t>
   </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
 </sst>
 </file>
 
@@ -271,7 +280,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,6 +476,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,7 +719,7 @@
     <xf numFmtId="38" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -731,6 +746,9 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1162,17 +1180,19 @@
   <dimension ref="B6:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="14.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.75" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="8" max="8" width="11.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9" style="1"/>
+    <col min="12" max="14" width="9" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:13">
@@ -1203,14 +1223,14 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="2:13" ht="14.45" customHeight="1">
+    <row r="8" spans="2:13" ht="14.4" customHeight="1">
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="8"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -1235,72 +1255,90 @@
       <c r="H9" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="J9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="2:13">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
     <row r="13" spans="2:13">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
     <row r="14" spans="2:13">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="2:13">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
     </row>
@@ -1312,17 +1350,25 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2">
+        <f>SUM(G10:G16)</f>
+        <v>0</v>
+      </c>
       <c r="H17" s="2"/>
+      <c r="J17" s="2"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
     </row>
@@ -1370,18 +1416,18 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="5.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="3:6" ht="25.5">
+    <row r="9" spans="3:6" ht="27.6">
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>

</xml_diff>